<commit_message>
Added graphs to experiments C and D
</commit_message>
<xml_diff>
--- a/experiments/2014-01-04/C1.xlsx
+++ b/experiments/2014-01-04/C1.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="960" yWindow="960" windowWidth="24640" windowHeight="18060" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="C1.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="C1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>0ft</t>
   </si>
@@ -41,13 +41,19 @@
   <si>
     <t>20ft</t>
   </si>
+  <si>
+    <t>25ft</t>
+  </si>
+  <si>
+    <t>30ft</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -102,7 +108,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -116,6 +122,192 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'C1'!$A$1:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'C1'!$I$1:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>54.91924074616914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.96460357428748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.755235074159449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.988530913495015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="463523592"/>
+        <c:axId val="463490728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="463523592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="463490728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="463490728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="463523592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I1" sqref="I1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -607,9 +799,26 @@
         <v>1.9885309134950155</v>
       </c>
     </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>